<commit_message>
Update placement algorithm, add Excel export, and optimize GA performance
</commit_message>
<xml_diff>
--- a/backend/output/results.xlsx
+++ b/backend/output/results.xlsx
@@ -719,7 +719,7 @@
         </is>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0.84</v>
+        <v>0.86</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>12</v>
@@ -758,7 +758,7 @@
         <v>100</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>6.857</v>
+        <v>6.429</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>5</v>
@@ -861,7 +861,7 @@
         <v>7.526</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>6.018</v>
+        <v>5.773</v>
       </c>
       <c r="I8" s="3" t="inlineStr">
         <is>
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="J8" s="2" t="n">
-        <v>1.79</v>
+        <v>1.82</v>
       </c>
       <c r="K8" s="2" t="n">
         <v>15</v>
@@ -908,10 +908,10 @@
         <v>100</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>7.5</v>
+        <v>7.208</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>6.133</v>
+        <v>6.039</v>
       </c>
       <c r="I9" s="3" t="inlineStr">
         <is>
@@ -919,7 +919,7 @@
         </is>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>15</v>
@@ -1008,10 +1008,10 @@
         <v>100</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>7.5</v>
+        <v>7.487</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>8.137</v>
+        <v>7.513</v>
       </c>
       <c r="I11" s="3" t="inlineStr">
         <is>
@@ -1019,7 +1019,7 @@
         </is>
       </c>
       <c r="J11" s="2" t="n">
-        <v>4.37</v>
+        <v>4.39</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>15</v>
@@ -1058,10 +1058,10 @@
         <v>100</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>7.775</v>
+        <v>5.3</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>7.4</v>
+        <v>7.5</v>
       </c>
       <c r="I12" s="3" t="inlineStr">
         <is>
@@ -1158,10 +1158,10 @@
         <v>100</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>9.077999999999999</v>
+        <v>9.664</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>7</v>
+        <v>7.047</v>
       </c>
       <c r="I14" s="3" t="inlineStr">
         <is>
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="J14" s="2" t="n">
-        <v>5.24</v>
+        <v>5.23</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>18</v>
@@ -1319,7 +1319,7 @@
         </is>
       </c>
       <c r="J17" s="2" t="n">
-        <v>15.4</v>
+        <v>15.46</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>20</v>
@@ -1458,10 +1458,10 @@
         <v>100</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>7.44</v>
+        <v>9.353999999999999</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>10.429</v>
+        <v>10.063</v>
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
@@ -1469,7 +1469,7 @@
         </is>
       </c>
       <c r="J20" s="2" t="n">
-        <v>11.75</v>
+        <v>11.94</v>
       </c>
       <c r="K20" s="2" t="n">
         <v>20</v>
@@ -1508,10 +1508,10 @@
         <v>100</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>10.026</v>
+        <v>8.888</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>9.541</v>
+        <v>10.011</v>
       </c>
       <c r="I21" s="3" t="inlineStr">
         <is>

</xml_diff>